<commit_message>
Allow comments in URL
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85615F9B-9009-4F12-A895-04838A7687C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C490D21-D97E-470B-ABB6-EC837DB95604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$3</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="83">
   <si>
     <t>URL</t>
   </si>
@@ -77,6 +77,201 @@
   </si>
   <si>
     <t>Regulation</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/reduce-post-consumer-waste/zoom-in</t>
+  </si>
+  <si>
+    <t>Tobacco Harm reduction</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products</t>
+  </si>
+  <si>
+    <t>Tobacco multi-product approach</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products/heated-tobacco-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/choice-diversity-of-adult-smokers-can-unlock-smoke-free-future</t>
+  </si>
+  <si>
+    <t>PMI Transformation</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/davos/davos-2019---rethinking-solutions-for-public-health</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/itstime/its-time-frequently-asked-questions</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/our-approach-to-sustainability/value-chain</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/demand-for-better-alternatives-to-smoking</t>
+  </si>
+  <si>
+    <t>Our science</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/the-problem-with-burning</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/about-us-faq</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/better-alternatives-to-smoking-explained</t>
+  </si>
+  <si>
+    <t>Investor Relations</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/key-milestones</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/glossary-section/glossary/alternatives-to-smoking</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/unsmoke-your-mind/time-for-conversations-what-can-we-achieve-together</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/inclusion-diversity/leveraging-the-talents-of-women/diversity-driving-change/annie-heremans</t>
+  </si>
+  <si>
+    <t>Inclusion, Diversity</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/suppliers/work-with-us-procurement</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/investor-relations/overview/building-leading-brands</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/leaders-of-change/stacey-kennedy-why-we-should-be-moving-forward-not-standing-still</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/case-studies-and-market-stories/human-rights-due-diligence-in-mexico</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/better/the-public-supports-governments-taking-a-new-approach-to-reducing-smoking-rates</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/realprogress/pmi-appeals-for-inclusive-public-engagement-to-address-the-greatest-problems-facing-our-society</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/heated-tobacco-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/low-carbon-transition-plan/driving-business-growth-forward-by-integrating-esg-factors</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/tobacco-harm-reduction/what-is-tobacco-harm-reduction</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/sustainability-news/dow-jones-sustainability-index-north-america-recognizes-pmi-s-sustainability-performance</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/careers/areas-of-work/operations</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products/e-vapor-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/prevent-youth-use-of-smoke-free-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/careers/make-history/philippines</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/smoke-free-life/youth-and-nicotine</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/davos/looking-back-on-davos</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/itstime/it's-time-to-start-a-conversation</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/integrated-report-2018/community</t>
+  </si>
+  <si>
+    <t>Partnership and Engagement</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/our-approach-to-sustainability/sustainability-resources</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/e-vapor</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/heated-tobacco-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/tobacco-harm-reduction/assessing-tobacco-risk-reduction</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/our-views-and-standards/our-views/underage-tobacco-and-nicotine-use</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/inclusion-diversity/leveraging-the-talents-of-women/diversity-driving-change/filiz-yavuz-diren</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/suppliers/sustainable-sourcing-for-suppliers</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/our-views-and-standards</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/investor-relations/press-releases-and-events/press-releases-overview</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/leaders-of-change/the-art-of-failing-a-key-to-success</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/inclusion-diversity/employee-resource-groups</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/realprogress/science-deserves-a-seat-at-the-table</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/smoking-and-cigarettes</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/low-carbon-transition-plan/harnessing-the-power-of-new-technologies-and-nature-based-solutions</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/letstalk/the-transformative-power-of-inclusion</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/sustainability-news/strategic-sustainability---why-transparent-reporting-matters</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/illicit-trade-prevention</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/us/campaigns/embrace-dialogue-to-disarm-hate/the-transformative-power-of-inclusion</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/careers/areas-of-work/product</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products/oral-smokeless-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/defining-smoke-free-products-eco-design-process</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/media-center/news/pmi-welcomes-the-forthcoming-entry-into-force-of-the-who-protocol-against-illicit-trade</t>
+  </si>
+  <si>
+    <t># from review</t>
+  </si>
+  <si>
+    <t># from previous run with score &gt; 0.5</t>
   </si>
 </sst>
 </file>
@@ -135,11 +330,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,11 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,43 +706,42 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -548,43 +749,662 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Apply priority for URL words. Add html classes for bs4.
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C490D21-D97E-470B-ABB6-EC837DB95604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B613CA-70C4-4361-8265-39712B48699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,27 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$67</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="83">
   <si>
     <t>URL</t>
   </si>
@@ -73,9 +86,6 @@
     <t>Leadership content</t>
   </si>
   <si>
-    <t>Tobacco harm reduction</t>
-  </si>
-  <si>
     <t>Regulation</t>
   </si>
   <si>
@@ -88,197 +98,200 @@
     <t>https://www.pmi.com/our-business/smoke-free-products</t>
   </si>
   <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products/heated-tobacco-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/choice-diversity-of-adult-smokers-can-unlock-smoke-free-future</t>
+  </si>
+  <si>
+    <t>PMI Transformation</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/davos/davos-2019---rethinking-solutions-for-public-health</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/itstime/its-time-frequently-asked-questions</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/our-approach-to-sustainability/value-chain</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/demand-for-better-alternatives-to-smoking</t>
+  </si>
+  <si>
+    <t>Our science</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/the-problem-with-burning</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/about-us-faq</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/better-alternatives-to-smoking-explained</t>
+  </si>
+  <si>
+    <t>Investor Relations</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/key-milestones</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/glossary-section/glossary/alternatives-to-smoking</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/unsmoke-your-mind/time-for-conversations-what-can-we-achieve-together</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/inclusion-diversity/leveraging-the-talents-of-women/diversity-driving-change/annie-heremans</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/suppliers/work-with-us-procurement</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/investor-relations/overview/building-leading-brands</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/leaders-of-change/stacey-kennedy-why-we-should-be-moving-forward-not-standing-still</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/case-studies-and-market-stories/human-rights-due-diligence-in-mexico</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/better/the-public-supports-governments-taking-a-new-approach-to-reducing-smoking-rates</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/realprogress/pmi-appeals-for-inclusive-public-engagement-to-address-the-greatest-problems-facing-our-society</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/heated-tobacco-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/low-carbon-transition-plan/driving-business-growth-forward-by-integrating-esg-factors</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/tobacco-harm-reduction/what-is-tobacco-harm-reduction</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/sustainability-news/dow-jones-sustainability-index-north-america-recognizes-pmi-s-sustainability-performance</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/careers/areas-of-work/operations</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products/e-vapor-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/prevent-youth-use-of-smoke-free-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/careers/make-history/philippines</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/smoke-free-life/youth-and-nicotine</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/davos/looking-back-on-davos</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-initiatives/itstime/it's-time-to-start-a-conversation</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/integrated-report-2018/community</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/our-approach-to-sustainability/sustainability-resources</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/e-vapor</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/heated-tobacco-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-science/tobacco-harm-reduction/assessing-tobacco-risk-reduction</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/our-views-and-standards/our-views/underage-tobacco-and-nicotine-use</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/inclusion-diversity/leveraging-the-talents-of-women/diversity-driving-change/filiz-yavuz-diren</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/suppliers/sustainable-sourcing-for-suppliers</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/our-views-and-standards</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/investor-relations/press-releases-and-events/press-releases-overview</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/leaders-of-change/the-art-of-failing-a-key-to-success</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/who-we-are/inclusion-diversity/employee-resource-groups</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/realprogress/science-deserves-a-seat-at-the-table</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/faq-section/smoking-and-cigarettes</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/low-carbon-transition-plan/harnessing-the-power-of-new-technologies-and-nature-based-solutions</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/letstalk/the-transformative-power-of-inclusion</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/sustainability/sustainability-news/strategic-sustainability---why-transparent-reporting-matters</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/illicit-trade-prevention</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/us/campaigns/embrace-dialogue-to-disarm-hate/the-transformative-power-of-inclusion</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/careers/areas-of-work/product</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-business/smoke-free-products/oral-smokeless-products</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/defining-smoke-free-products-eco-design-process</t>
+  </si>
+  <si>
+    <t>https://www.pmi.com/media-center/news/pmi-welcomes-the-forthcoming-entry-into-force-of-the-who-protocol-against-illicit-trade</t>
+  </si>
+  <si>
+    <t>Our Science</t>
+  </si>
+  <si>
+    <t>Investor relations</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t># from review 26 Sept 2023</t>
+  </si>
+  <si>
+    <t>Inclusion, Diversity</t>
+  </si>
+  <si>
     <t>Tobacco multi-product approach</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-business/smoke-free-products/heated-tobacco-products</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/choice-diversity-of-adult-smokers-can-unlock-smoke-free-future</t>
-  </si>
-  <si>
-    <t>PMI Transformation</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-initiatives/davos/davos-2019---rethinking-solutions-for-public-health</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-initiatives/itstime/its-time-frequently-asked-questions</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/our-approach-to-sustainability/value-chain</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-science/demand-for-better-alternatives-to-smoking</t>
-  </si>
-  <si>
-    <t>Our science</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-science/the-problem-with-burning</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/faq-section/about-us-faq</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/better-alternatives-to-smoking-explained</t>
-  </si>
-  <si>
-    <t>Investor Relations</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/who-we-are/key-milestones</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/glossary-section/glossary/alternatives-to-smoking</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-initiatives/unsmoke-your-mind/time-for-conversations-what-can-we-achieve-together</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/who-we-are/inclusion-diversity/leveraging-the-talents-of-women/diversity-driving-change/annie-heremans</t>
-  </si>
-  <si>
-    <t>Inclusion, Diversity</t>
-  </si>
-  <si>
-    <t>Jobs</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-business/suppliers/work-with-us-procurement</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/investor-relations/overview/building-leading-brands</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-transformation/leaders-of-change/stacey-kennedy-why-we-should-be-moving-forward-not-standing-still</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/case-studies-and-market-stories/human-rights-due-diligence-in-mexico</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/better/the-public-supports-governments-taking-a-new-approach-to-reducing-smoking-rates</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/realprogress/pmi-appeals-for-inclusive-public-engagement-to-address-the-greatest-problems-facing-our-society</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/faq-section/heated-tobacco-products</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/low-carbon-transition-plan/driving-business-growth-forward-by-integrating-esg-factors</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-science/tobacco-harm-reduction/what-is-tobacco-harm-reduction</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/sustainability-news/dow-jones-sustainability-index-north-america-recognizes-pmi-s-sustainability-performance</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/careers/areas-of-work/operations</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-business/smoke-free-products/e-vapor-products</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/prevent-youth-use-of-smoke-free-products</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/careers/make-history/philippines</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/smoke-free-life/youth-and-nicotine</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-initiatives/davos/looking-back-on-davos</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-initiatives/itstime/it's-time-to-start-a-conversation</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/integrated-report-2018/community</t>
-  </si>
-  <si>
-    <t>Partnership and Engagement</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/our-approach-to-sustainability/sustainability-resources</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/faq-section/e-vapor</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-science/heated-tobacco-products</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-science/tobacco-harm-reduction/assessing-tobacco-risk-reduction</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/who-we-are/our-views-and-standards/our-views/underage-tobacco-and-nicotine-use</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/who-we-are/inclusion-diversity/leveraging-the-talents-of-women/diversity-driving-change/filiz-yavuz-diren</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-business/suppliers/sustainable-sourcing-for-suppliers</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/who-we-are/our-views-and-standards</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/investor-relations/press-releases-and-events/press-releases-overview</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-transformation/leaders-of-change/the-art-of-failing-a-key-to-success</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/who-we-are/inclusion-diversity/employee-resource-groups</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/realprogress/science-deserves-a-seat-at-the-table</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/faq-section/smoking-and-cigarettes</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/low-carbon-transition-plan/harnessing-the-power-of-new-technologies-and-nature-based-solutions</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/letstalk/the-transformative-power-of-inclusion</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/sustainability/sustainability-news/strategic-sustainability---why-transparent-reporting-matters</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-business/illicit-trade-prevention</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/us/campaigns/embrace-dialogue-to-disarm-hate/the-transformative-power-of-inclusion</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/careers/areas-of-work/product</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-business/smoke-free-products/oral-smokeless-products</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-transformation/pmis-multi-category-approach-toward-a-smoke-free-future/defining-smoke-free-products-eco-design-process</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/media-center/news/pmi-welcomes-the-forthcoming-entry-into-force-of-the-who-protocol-against-illicit-trade</t>
-  </si>
-  <si>
-    <t># from review</t>
-  </si>
-  <si>
-    <t># from previous run with score &gt; 0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +303,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -341,7 +368,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,11 +708,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +735,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -716,8 +744,11 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -725,10 +756,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -736,7 +767,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -746,6 +780,9 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -754,6 +791,9 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -770,18 +810,33 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -789,23 +844,32 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>82</v>
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -813,21 +877,21 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -835,43 +899,43 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -879,32 +943,32 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -912,40 +976,40 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -956,62 +1020,62 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
         <v>13</v>
@@ -1019,186 +1083,174 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" t="s">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" t="s">
-        <v>13</v>
+        <v>82</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
@@ -1206,142 +1258,142 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C63" t="s">
         <v>13</v>
@@ -1349,61 +1401,50 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C64" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C65" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" t="s">
         <v>79</v>
       </c>
-      <c r="B67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added hardcoded rule for 'written by' Fix Golden data.
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F3D4B2-77BB-40AF-8583-6B7FB8F217E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2BFE40-AE72-4750-8F93-1B38864326F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="82">
   <si>
     <t>URL</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>https://www.pmi.com/media-center/news/wearesmokefree</t>
-  </si>
-  <si>
-    <t>https://www.pmi.com/our-initiatives/cannes-lion-2019/the-facts-why-we-are-in-cannes</t>
   </si>
   <si>
     <t>https://www.pmi.com/our-initiatives/veterans</t>
@@ -667,11 +664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -708,10 +705,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -719,10 +716,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,10 +727,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -741,10 +738,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -752,10 +749,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -763,10 +760,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -774,10 +771,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -785,32 +782,32 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,10 +815,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -829,21 +826,21 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -851,10 +848,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -862,10 +859,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -873,21 +870,21 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -895,10 +892,10 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -906,21 +903,21 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -928,10 +925,10 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -939,10 +936,10 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -950,21 +947,21 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>18</v>
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
         <v>13</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -972,10 +969,10 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -983,21 +980,19 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1005,10 +1000,10 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
         <v>14</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1016,10 +1011,10 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1027,43 +1022,43 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" t="s">
-        <v>18</v>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>15</v>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>18</v>
+      <c r="B35" t="s">
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1071,10 +1066,10 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1082,32 +1077,32 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
+        <v>80</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="B38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>18</v>
+      <c r="B38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>16</v>
+      <c r="B39" t="s">
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1115,10 +1110,10 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1126,32 +1121,32 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>52</v>
       </c>
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" t="s">
-        <v>15</v>
+      <c r="B42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>16</v>
+      <c r="B43" t="s">
+        <v>13</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1159,21 +1154,21 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>82</v>
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>55</v>
       </c>
-      <c r="B45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" t="s">
-        <v>31</v>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1181,10 +1176,10 @@
         <v>56</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1192,21 +1187,21 @@
         <v>57</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>27</v>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1214,10 +1209,10 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1225,10 +1220,10 @@
         <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1236,10 +1231,10 @@
         <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>82</v>
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1247,10 +1242,10 @@
         <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1258,10 +1253,10 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1269,10 +1264,10 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" t="s">
-        <v>22</v>
+        <v>79</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1280,10 +1275,10 @@
         <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1291,10 +1286,10 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="C56" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1302,10 +1297,10 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1313,10 +1308,10 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1324,32 +1319,32 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>70</v>
       </c>
-      <c r="B60" t="s">
-        <v>14</v>
+      <c r="B60" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>16</v>
+      <c r="B61" t="s">
+        <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1357,10 +1352,10 @@
         <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C62" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1368,10 +1363,10 @@
         <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1379,10 +1374,10 @@
         <v>74</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1390,25 +1385,14 @@
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C66" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Extended html parser. Fix description of Leadership content Fix golden data
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2BFE40-AE72-4750-8F93-1B38864326F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F93D860-BE3A-4E53-BAA4-F1BFF0948D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,10 +749,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -782,10 +782,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -793,10 +793,10 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1000,10 +1000,10 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,11 +1032,11 @@
       <c r="A33" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1121,10 +1121,10 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1209,10 +1209,10 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
         <v>79</v>
-      </c>
-      <c r="C49" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1275,10 +1275,10 @@
         <v>65</v>
       </c>
       <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" t="s">
         <v>26</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1297,10 +1297,10 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="s">
         <v>13</v>
-      </c>
-      <c r="C57" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add counter of leaders in text ref.
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F93D860-BE3A-4E53-BAA4-F1BFF0948D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60618944-EDF6-443D-A57F-662C689286AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,13 +353,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,7 +670,7 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -999,8 +1002,8 @@
       <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" t="s">
-        <v>14</v>
+      <c r="B30" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Whitelist and blacklist of classes.
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60618944-EDF6-443D-A57F-662C689286AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8557597-97B5-4025-8514-397CC86D9AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,8 +670,8 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,10 +1311,10 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" t="s">
         <v>79</v>
-      </c>
-      <c r="C58" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1322,10 +1322,10 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" t="s">
         <v>13</v>
-      </c>
-      <c r="C59" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1344,10 +1344,10 @@
         <v>71</v>
       </c>
       <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" t="s">
         <v>79</v>
-      </c>
-      <c r="C61" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add new classes. Fix golden data.
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D60EBC-CA83-43EE-8E99-26EDA2903B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307BA914-3C2E-4B09-98E4-EF94935B74A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,8 +670,8 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,10 +774,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -992,7 +992,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Fix topic description. Fix GD.
</commit_message>
<xml_diff>
--- a/golden-data/golden_data.xlsx
+++ b/golden-data/golden_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GptPOCs\PMI\sources\golden-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307BA914-3C2E-4B09-98E4-EF94935B74A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF7A55-EF95-4774-BC2A-18D012C27C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,11 +667,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -703,7 +704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -714,7 +715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +726,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -736,7 +737,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -747,7 +748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -769,7 +770,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -780,7 +781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -791,7 +792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -802,7 +803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -813,7 +814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -824,7 +825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -835,7 +836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -846,7 +847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -857,7 +858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -868,7 +869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -879,7 +880,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -890,7 +891,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -901,7 +902,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -912,7 +913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -923,7 +924,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -934,7 +935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -945,7 +946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -967,7 +968,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -978,7 +979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -995,10 +996,10 @@
         <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1042,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -1270,10 +1271,10 @@
         <v>79</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -1317,7 +1318,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>73</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -1395,7 +1396,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C65" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Partnership and Engagement"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>